<commit_message>
More info on Cabrillo freeway flyers
</commit_message>
<xml_diff>
--- a/cabrillo-freeway/cabrillo-freeway-flyers-fuzzy-match.xlsx
+++ b/cabrillo-freeway/cabrillo-freeway-flyers-fuzzy-match.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laptopuser/Dropbox/teaching/www/ccc-salary-study/cabrillo-freeway/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{2FAB9C48-2F4C-8D48-A395-9360B4D36E6A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EA3E6AA3-A02F-4A41-84BC-89BC9B8B8888}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cabrillo-freeway-flyers-fuzzy-m" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="118">
   <si>
     <t>Employee Name</t>
   </si>
@@ -376,12 +376,15 @@
   </si>
   <si>
     <t>&lt;$25K</t>
+  </si>
+  <si>
+    <t>&gt;$50K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -934,7 +937,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43264.831664351848" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="149">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43264.831664351848" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="149" xr:uid="{00000000-000A-0000-FFFF-FFFF0D000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:L1048576" sheet="cabrillo-freeway-flyers-fuzzy-m"/>
   </cacheSource>
@@ -3146,7 +3149,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -3758,10 +3761,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+    <sheetView topLeftCell="A131" workbookViewId="0">
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
@@ -8569,7 +8572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:B71"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
@@ -9138,11 +9141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9292,6 +9295,17 @@
       <c r="B10" s="2">
         <v>26203.75</v>
       </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10">
+        <f>COUNTIF(B:B, "&gt;50000")</f>
+        <v>26</v>
+      </c>
+      <c r="F10" s="4">
+        <f>E10/E1</f>
+        <v>0.39393939393939392</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">

</xml_diff>